<commit_message>
fix import and export for asset
</commit_message>
<xml_diff>
--- a/public/DataAset/data-aset.xlsx
+++ b/public/DataAset/data-aset.xlsx
@@ -5,22 +5,35 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fikar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\udhel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCCE5B9-3947-4808-95BA-ED3AAD6F12DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BB102F-9991-4A43-B4CA-6100B32F6DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4284" yWindow="2952" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>No</t>
   </si>
@@ -73,9 +86,15 @@
     <t>Vendor</t>
   </si>
   <si>
+    <t>Komputer</t>
+  </si>
+  <si>
     <t>unit</t>
   </si>
   <si>
+    <t>01/06/2023</t>
+  </si>
+  <si>
     <t>Testing</t>
   </si>
   <si>
@@ -91,22 +110,13 @@
     <t>y</t>
   </si>
   <si>
+    <t>Bangunan dan Prasarana</t>
+  </si>
+  <si>
     <t>Belum Terisi</t>
   </si>
   <si>
-    <t>Laboratorium Instalasi Tenaga Listrik</t>
-  </si>
-  <si>
-    <t>0001/MP/SA/LITL</t>
-  </si>
-  <si>
-    <t>Chain</t>
-  </si>
-  <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>Mesin dan Peralatan</t>
+    <t>Informatics</t>
   </si>
 </sst>
 </file>
@@ -152,15 +162,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -467,32 +474,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="69.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="47" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,66 +551,56 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>25</v>
+      <c r="B2" s="2">
+        <v>9099203</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="3">
-        <v>45388</v>
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="2">
-        <v>11223455</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mengembalikan direksi, dan membuat upload hanya bisa jpg, jpeg, dan png
</commit_message>
<xml_diff>
--- a/public/DataAset/data-aset.xlsx
+++ b/public/DataAset/data-aset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\udhel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yusuf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BB102F-9991-4A43-B4CA-6100B32F6DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073628AF-FA63-43FA-B522-1A4E37BA1F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>No</t>
   </si>
@@ -86,37 +86,85 @@
     <t>Vendor</t>
   </si>
   <si>
-    <t>Komputer</t>
+    <t>0001/PK/SS/GA</t>
+  </si>
+  <si>
+    <t>ASUS ROG</t>
   </si>
   <si>
     <t>unit</t>
   </si>
   <si>
-    <t>01/06/2023</t>
-  </si>
-  <si>
-    <t>Testing</t>
+    <t>13/02/2018</t>
+  </si>
+  <si>
+    <t>{"id":2,"name":"ASUS","created_at":"2024-10-27T07:43:08.000000Z","updated_at":"2024-10-27T07:43:08.000000Z"}</t>
   </si>
   <si>
     <t>Baik</t>
   </si>
   <si>
-    <t>gambar_aset/monitor.jpg</t>
-  </si>
-  <si>
-    <t>testing</t>
+    <t>gambar_user/Kz5QfJAOnWwgQR9dq0w6eJBtOQWNOiC1P4jPy3lB.png</t>
+  </si>
+  <si>
+    <t>amin</t>
+  </si>
+  <si>
+    <t>digudang</t>
   </si>
   <si>
     <t>y</t>
   </si>
   <si>
-    <t>Bangunan dan Prasarana</t>
-  </si>
-  <si>
-    <t>Belum Terisi</t>
-  </si>
-  <si>
-    <t>Informatics</t>
+    <t>Peralatan Kantor</t>
+  </si>
+  <si>
+    <t>Belum Ada</t>
+  </si>
+  <si>
+    <t>GEDUNG A5</t>
+  </si>
+  <si>
+    <t>Sejahtera Sukma</t>
+  </si>
+  <si>
+    <t>0001/PK/IV/GA</t>
+  </si>
+  <si>
+    <t>MSI CYBORG</t>
+  </si>
+  <si>
+    <t>14/10/2024</t>
+  </si>
+  <si>
+    <t>{"id":4,"name":"MSI","created_at":"2024-10-27T07:45:23.000000Z","updated_at":"2024-10-27T07:47:08.000000Z"}</t>
+  </si>
+  <si>
+    <t>gambar_user/Kq3oj51MfVgd3FgwXVLOGAwmoHsjYrc1cITHjYnM.png</t>
+  </si>
+  <si>
+    <t>marzuki</t>
+  </si>
+  <si>
+    <t>Tanpa Pemeliharaan</t>
+  </si>
+  <si>
+    <t>International Vender</t>
+  </si>
+  <si>
+    <t>0002/PK/SS/GA</t>
+  </si>
+  <si>
+    <t>ASUS ZEPY</t>
+  </si>
+  <si>
+    <t>ASUS</t>
+  </si>
+  <si>
+    <t>Amin</t>
+  </si>
+  <si>
+    <t>Jon.jpg</t>
   </si>
 </sst>
 </file>
@@ -162,12 +210,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -474,31 +525,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="130.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="69.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,54 +604,163 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>9099203</v>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2">
+        <v>221333786900</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="L3" s="2">
+        <v>21314435235</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="N3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44844</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="2">
+        <v>22133412</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>